<commit_message>
Fix distribution issue (where `mcr ` wasn't counted as selfish)
</commit_message>
<xml_diff>
--- a/MCR_Analysis/RuleTables.xlsx
+++ b/MCR_Analysis/RuleTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby Ford\Desktop\ecoli_amr_persistence\MCR_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8557FDB8-AC10-4319-BC25-A8EDA5449119}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714E068C-4994-4DAF-BEB8-2C89444FFAF2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E9B528E1-14AB-40D2-991D-A32EC9F727BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E9B528E1-14AB-40D2-991D-A32EC9F727BC}"/>
   </bookViews>
   <sheets>
     <sheet name="ARM_Training" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="95">
   <si>
     <t>ID</t>
   </si>
@@ -44,9 +44,6 @@
     <t>RHS</t>
   </si>
   <si>
-    <t>Rule Size</t>
-  </si>
-  <si>
     <t>Support</t>
   </si>
   <si>
@@ -296,9 +293,6 @@
     <t>aac(3)-IId,blaCTX-M-55,blaEC,qnrS1,tet(A)</t>
   </si>
   <si>
-    <t>aadA1,aph(3')-IIa,blaEC,blaTEM-1,bleO,qacEdelta1,sul1,tet(A)</t>
-  </si>
-  <si>
     <t>aadA1,arr-2,blaEC,blaOXA-10,cmlA5,dfrA14,qnrS1,tet(A)</t>
   </si>
   <si>
@@ -314,9 +308,6 @@
     <t>aac(3)-IId,aadA5,aph(3'')-Ib,aph(6)-Id,blaCTX-M-65,blaEC,blaTEM-1,dfrA17,erm(B),fosA3,mph(A),qacEdelta1,sul1,sul2,tet(A)</t>
   </si>
   <si>
-    <t>aac(3)-IId,aadA1,aadA2,aadA5,aph(3'')-Ib,aph(3')-IIa,aph(6)-Id,blaCTX-M-55,blaEC,blaNDM-5,blaTEM-1,ble,bleO,cmlA1,dfrA17,floR,mph(A),qacE,qacL,sul1,sul2,sul3,tet(A)</t>
-  </si>
-  <si>
     <t>Gene Set</t>
   </si>
   <si>
@@ -324,6 +315,9 @@
   </si>
   <si>
     <t>SMOTE Odds Ratio</t>
+  </si>
+  <si>
+    <t>Set Size</t>
   </si>
 </sst>
 </file>
@@ -333,7 +327,14 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,15 +360,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -681,7 +685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08EB49E5-2606-48E5-A9C1-3CDA8661D6AA}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection sqref="A1:H47"/>
     </sheetView>
   </sheetViews>
@@ -690,7 +694,7 @@
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="77.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -704,19 +708,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
+      <c r="H1" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -724,10 +728,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -741,7 +745,7 @@
       <c r="G2">
         <v>108</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>0.375</v>
       </c>
     </row>
@@ -750,10 +754,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -767,7 +771,7 @@
       <c r="G3">
         <v>119</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>0.625</v>
       </c>
     </row>
@@ -776,10 +780,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -793,7 +797,7 @@
       <c r="G4">
         <v>114</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <v>0.75</v>
       </c>
     </row>
@@ -802,10 +806,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>8</v>
@@ -819,7 +823,7 @@
       <c r="G5">
         <v>110</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="2">
         <v>0.5</v>
       </c>
     </row>
@@ -828,10 +832,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>8</v>
@@ -845,7 +849,7 @@
       <c r="G6">
         <v>108</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="2">
         <v>0.5</v>
       </c>
     </row>
@@ -854,10 +858,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>8</v>
@@ -871,7 +875,7 @@
       <c r="G7">
         <v>106</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="2">
         <v>0.625</v>
       </c>
     </row>
@@ -880,10 +884,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>9</v>
@@ -897,7 +901,7 @@
       <c r="G8">
         <v>91</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="2">
         <v>0.44444440000000002</v>
       </c>
     </row>
@@ -906,10 +910,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <v>9</v>
@@ -923,7 +927,7 @@
       <c r="G9">
         <v>79</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <v>0.44444440000000002</v>
       </c>
     </row>
@@ -932,10 +936,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -949,7 +953,7 @@
       <c r="G10">
         <v>80</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="2">
         <v>0.44444440000000002</v>
       </c>
     </row>
@@ -958,10 +962,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>9</v>
@@ -975,7 +979,7 @@
       <c r="G11">
         <v>78</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="2">
         <v>0.55555560000000004</v>
       </c>
     </row>
@@ -984,10 +988,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12">
         <v>9</v>
@@ -1001,7 +1005,7 @@
       <c r="G12">
         <v>103</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="2">
         <v>0.66666669999999995</v>
       </c>
     </row>
@@ -1010,10 +1014,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>9</v>
@@ -1027,7 +1031,7 @@
       <c r="G13">
         <v>90</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="2">
         <v>0.55555560000000004</v>
       </c>
     </row>
@@ -1036,10 +1040,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14">
         <v>10</v>
@@ -1053,7 +1057,7 @@
       <c r="G14">
         <v>66</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="2">
         <v>0.6</v>
       </c>
     </row>
@@ -1062,10 +1066,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -1079,7 +1083,7 @@
       <c r="G15">
         <v>67</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="2">
         <v>0.5</v>
       </c>
     </row>
@@ -1088,10 +1092,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -1105,7 +1109,7 @@
       <c r="G16">
         <v>64</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="2">
         <v>0.5</v>
       </c>
     </row>
@@ -1114,10 +1118,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17">
         <v>10</v>
@@ -1131,7 +1135,7 @@
       <c r="G17">
         <v>65</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="2">
         <v>0.5</v>
       </c>
     </row>
@@ -1140,10 +1144,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <v>10</v>
@@ -1157,7 +1161,7 @@
       <c r="G18">
         <v>66</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="2">
         <v>0.6</v>
       </c>
     </row>
@@ -1166,10 +1170,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19">
         <v>10</v>
@@ -1183,7 +1187,7 @@
       <c r="G19">
         <v>67</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="2">
         <v>0.6</v>
       </c>
     </row>
@@ -1192,10 +1196,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -1209,7 +1213,7 @@
       <c r="G20">
         <v>66</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="2">
         <v>0.7</v>
       </c>
     </row>
@@ -1218,10 +1222,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21">
         <v>10</v>
@@ -1235,7 +1239,7 @@
       <c r="G21">
         <v>66</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="2">
         <v>0.5</v>
       </c>
     </row>
@@ -1244,10 +1248,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22">
         <v>11</v>
@@ -1261,7 +1265,7 @@
       <c r="G22">
         <v>46</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="2">
         <v>0.36363640000000003</v>
       </c>
     </row>
@@ -1270,10 +1274,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23">
         <v>11</v>
@@ -1287,7 +1291,7 @@
       <c r="G23">
         <v>51</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="2">
         <v>0.54545449999999995</v>
       </c>
     </row>
@@ -1296,10 +1300,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24">
         <v>11</v>
@@ -1313,7 +1317,7 @@
       <c r="G24">
         <v>49</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="2">
         <v>0.63636360000000003</v>
       </c>
     </row>
@@ -1322,10 +1326,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25">
         <v>11</v>
@@ -1339,7 +1343,7 @@
       <c r="G25">
         <v>47</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="2">
         <v>0.72727269999999999</v>
       </c>
     </row>
@@ -1348,10 +1352,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26">
         <v>11</v>
@@ -1365,7 +1369,7 @@
       <c r="G26">
         <v>51</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="2">
         <v>0.63636360000000003</v>
       </c>
     </row>
@@ -1374,10 +1378,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27">
         <v>11</v>
@@ -1391,7 +1395,7 @@
       <c r="G27">
         <v>48</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="2">
         <v>0.63636360000000003</v>
       </c>
     </row>
@@ -1400,10 +1404,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28">
         <v>11</v>
@@ -1417,7 +1421,7 @@
       <c r="G28">
         <v>53</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="2">
         <v>0.54545449999999995</v>
       </c>
     </row>
@@ -1426,10 +1430,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29">
         <v>11</v>
@@ -1443,7 +1447,7 @@
       <c r="G29">
         <v>49</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="2">
         <v>0.63636360000000003</v>
       </c>
     </row>
@@ -1452,10 +1456,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D30">
         <v>11</v>
@@ -1469,7 +1473,7 @@
       <c r="G30">
         <v>49</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="2">
         <v>0.54545449999999995</v>
       </c>
     </row>
@@ -1478,10 +1482,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31">
         <v>11</v>
@@ -1495,7 +1499,7 @@
       <c r="G31">
         <v>46</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31" s="2">
         <v>0.54545449999999995</v>
       </c>
     </row>
@@ -1504,10 +1508,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32">
         <v>11</v>
@@ -1521,7 +1525,7 @@
       <c r="G32">
         <v>46</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H32" s="2">
         <v>0.72727269999999999</v>
       </c>
     </row>
@@ -1530,10 +1534,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D33">
         <v>11</v>
@@ -1547,7 +1551,7 @@
       <c r="G33">
         <v>54</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H33" s="2">
         <v>0.63636360000000003</v>
       </c>
     </row>
@@ -1556,10 +1560,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D34">
         <v>11</v>
@@ -1573,7 +1577,7 @@
       <c r="G34">
         <v>47</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H34" s="2">
         <v>0.72727269999999999</v>
       </c>
     </row>
@@ -1582,10 +1586,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D35">
         <v>11</v>
@@ -1599,7 +1603,7 @@
       <c r="G35">
         <v>46</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H35" s="2">
         <v>0.54545449999999995</v>
       </c>
     </row>
@@ -1608,10 +1612,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D36">
         <v>11</v>
@@ -1625,7 +1629,7 @@
       <c r="G36">
         <v>53</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H36" s="2">
         <v>0.63636360000000003</v>
       </c>
     </row>
@@ -1634,10 +1638,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37">
         <v>11</v>
@@ -1651,7 +1655,7 @@
       <c r="G37">
         <v>46</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H37" s="2">
         <v>0.54545449999999995</v>
       </c>
     </row>
@@ -1660,10 +1664,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D38">
         <v>11</v>
@@ -1677,7 +1681,7 @@
       <c r="G38">
         <v>49</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H38" s="2">
         <v>0.54545449999999995</v>
       </c>
     </row>
@@ -1686,10 +1690,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D39">
         <v>11</v>
@@ -1703,7 +1707,7 @@
       <c r="G39">
         <v>47</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H39" s="2">
         <v>0.54545449999999995</v>
       </c>
     </row>
@@ -1712,10 +1716,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D40">
         <v>11</v>
@@ -1729,7 +1733,7 @@
       <c r="G40">
         <v>49</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H40" s="2">
         <v>0.45454549999999999</v>
       </c>
     </row>
@@ -1738,10 +1742,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D41">
         <v>11</v>
@@ -1755,7 +1759,7 @@
       <c r="G41">
         <v>51</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H41" s="2">
         <v>0.54545449999999995</v>
       </c>
     </row>
@@ -1764,10 +1768,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42">
         <v>11</v>
@@ -1781,7 +1785,7 @@
       <c r="G42">
         <v>56</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H42" s="2">
         <v>0.54545449999999995</v>
       </c>
     </row>
@@ -1790,10 +1794,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D43">
         <v>11</v>
@@ -1807,7 +1811,7 @@
       <c r="G43">
         <v>57</v>
       </c>
-      <c r="H43" s="1">
+      <c r="H43" s="2">
         <v>0.63636360000000003</v>
       </c>
     </row>
@@ -1816,10 +1820,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D44">
         <v>11</v>
@@ -1833,7 +1837,7 @@
       <c r="G44">
         <v>46</v>
       </c>
-      <c r="H44" s="1">
+      <c r="H44" s="2">
         <v>0.45454549999999999</v>
       </c>
     </row>
@@ -1842,10 +1846,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D45">
         <v>13</v>
@@ -1859,7 +1863,7 @@
       <c r="G45">
         <v>35</v>
       </c>
-      <c r="H45" s="1">
+      <c r="H45" s="2">
         <v>0.3846154</v>
       </c>
     </row>
@@ -1868,10 +1872,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D46">
         <v>13</v>
@@ -1885,7 +1889,7 @@
       <c r="G46">
         <v>34</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H46" s="2">
         <v>0.61538459999999995</v>
       </c>
     </row>
@@ -1894,10 +1898,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D47">
         <v>13</v>
@@ -1911,7 +1915,7 @@
       <c r="G47">
         <v>34</v>
       </c>
-      <c r="H47" s="1">
+      <c r="H47" s="2">
         <v>0.53846099999999997</v>
       </c>
     </row>
@@ -1925,7 +1929,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,7 +1944,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1949,16 +1953,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1966,10 +1970,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -1989,10 +1993,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -2012,10 +2016,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -2035,10 +2039,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>8</v>
@@ -2058,10 +2062,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>8</v>
@@ -2081,10 +2085,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>8</v>
@@ -2104,10 +2108,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>9</v>
@@ -2127,10 +2131,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <v>9</v>
@@ -2150,10 +2154,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -2173,10 +2177,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>9</v>
@@ -2196,10 +2200,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -2219,10 +2223,10 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -2242,10 +2246,10 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14">
         <v>10</v>
@@ -2265,10 +2269,10 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -2288,10 +2292,10 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -2311,10 +2315,10 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17">
         <v>11</v>
@@ -2334,10 +2338,10 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <v>11</v>
@@ -2357,10 +2361,10 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19">
         <v>11</v>
@@ -2380,10 +2384,10 @@
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20">
         <v>11</v>
@@ -2403,10 +2407,10 @@
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21">
         <v>11</v>
@@ -2426,10 +2430,10 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22">
         <v>11</v>
@@ -2449,10 +2453,10 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23">
         <v>11</v>
@@ -2472,10 +2476,10 @@
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24">
         <v>11</v>
@@ -2495,10 +2499,10 @@
         <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25">
         <v>11</v>
@@ -2518,10 +2522,10 @@
         <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26">
         <v>11</v>
@@ -2541,10 +2545,10 @@
         <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27">
         <v>11</v>
@@ -2564,10 +2568,10 @@
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28">
         <v>13</v>
@@ -2587,10 +2591,10 @@
         <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29">
         <v>13</v>
@@ -2612,10 +2616,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF152AE1-04E6-4FF7-9B36-6A3314C85CB7}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B25"/>
+      <selection sqref="A1:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2623,412 +2627,614 @@
     <col min="1" max="1" width="165.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
         <v>94</v>
       </c>
-      <c r="B1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2">
+        <v>6.6944744089835702</v>
+      </c>
+      <c r="C2">
+        <v>17.655817073183901</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3">
+        <v>3.3677537110651201</v>
+      </c>
+      <c r="C3">
+        <v>6.9804810086311804</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4">
+        <v>3.9417535506930599</v>
+      </c>
+      <c r="C4">
+        <v>5.7439522526124502</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>4.7760109777618602</v>
+      </c>
+      <c r="C5">
+        <v>5.0773898509553597</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6">
+        <v>4.7708131418768396</v>
+      </c>
+      <c r="C6">
+        <v>4.9939617914307401</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="1">
-        <v>6.6944744089835702</v>
-      </c>
-      <c r="C2" s="1">
-        <v>17.655817073183901</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B7">
+        <v>2.3144028057267101</v>
+      </c>
+      <c r="C7">
+        <v>4.1365557992192103</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.42857142857142899</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8">
+        <v>4.1247172070595601</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>3.89305555281548</v>
+      </c>
+      <c r="C9">
+        <v>3.8623719658782698</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="1">
-        <v>4.7760109777618602</v>
-      </c>
-      <c r="C3" s="1">
-        <v>5.0773898509553597</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B10">
+        <v>2.2480435558445402</v>
+      </c>
+      <c r="C10">
+        <v>3.06137134315333</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11">
+        <v>2.8762574106171002</v>
+      </c>
+      <c r="C11">
+        <v>3.0492056204488098</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12">
+        <v>2.3017252713169598</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.53333333333333299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="1">
-        <v>4.7708131418768396</v>
-      </c>
-      <c r="C4" s="1">
-        <v>4.9939617914307401</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3.9417535506930599</v>
-      </c>
-      <c r="C5" s="1">
-        <v>5.7439522526124502</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B13">
+        <v>2.5135388103027698</v>
+      </c>
+      <c r="C13">
+        <v>2.28654568308967</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14">
+        <v>1.8470521143276399</v>
+      </c>
+      <c r="C14">
+        <v>2.1280851209562099</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15">
+        <v>1.9879225691309099</v>
+      </c>
+      <c r="D15">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.36363636363636398</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16">
+        <v>1.6456524645719099</v>
+      </c>
+      <c r="C16">
+        <v>1.9241042102039201</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17">
+        <v>1.50894175636454</v>
+      </c>
+      <c r="C17">
+        <v>1.6695214934409499</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18">
+        <v>1.3759093949209</v>
+      </c>
+      <c r="C18">
+        <v>1.57030608963531</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19">
+        <v>1.06606395986014</v>
+      </c>
+      <c r="C19">
+        <v>1.5478802937051801</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20">
+        <v>1.53282082393621</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21">
+        <v>1.4201301937451201</v>
+      </c>
+      <c r="D21">
+        <v>9</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.55555555555555602</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22">
+        <v>1.3218841303211499</v>
+      </c>
+      <c r="C22">
+        <v>1.3690174162493001</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23">
+        <v>1.1311208463048801</v>
+      </c>
+      <c r="C23">
+        <v>1.3404605989048799</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="1">
-        <v>3.89305555281548</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3.8623719658782698</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3.3677537110651201</v>
-      </c>
-      <c r="C7" s="1">
-        <v>6.9804810086311804</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2.8762574106171002</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3.0492056204488098</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2.5135388103027698</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2.28654568308967</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B24">
+        <v>1.2924825949173799</v>
+      </c>
+      <c r="C24">
+        <v>1.33898716281177</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25">
+        <v>1.2853214624389999</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26">
+        <v>1.6482885286432201</v>
+      </c>
+      <c r="C26">
+        <v>1.2199729476010801</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27">
+        <v>1.2171219834114699</v>
+      </c>
+      <c r="D27">
+        <v>14</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28">
+        <v>1.20866743770415</v>
+      </c>
+      <c r="C28">
+        <v>1.1651028095365701</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29">
+        <v>1.1633175016633599</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30">
+        <v>1.0761014631298</v>
+      </c>
+      <c r="C30">
+        <v>1.1392309384729999</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31">
+        <v>1.1390817646872</v>
+      </c>
+      <c r="C31">
+        <v>1.1249215439065601</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32">
+        <v>1.13900141343992</v>
+      </c>
+      <c r="C32">
+        <v>1.0912231451293599</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.71428571428571397</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33">
+        <v>1.01965479728596</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34">
+        <v>1.0170810789507501</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35">
+        <v>1.0562719363651401</v>
+      </c>
+      <c r="C35">
+        <v>1.01422823626237</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="1">
-        <v>2.3144028057267101</v>
-      </c>
-      <c r="C10" s="1">
-        <v>4.1365557992192103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2.2480435558445402</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3.06137134315333</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1.8470521143276399</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2.1280851209562099</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1.6482885286432201</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1.2199729476010801</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1.6456524645719099</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1.9241042102039201</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1.50894175636454</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1.6695214934409499</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1.3759093949209</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1.57030608963531</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1.3218841303211499</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1.3690174162493001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1.2924825949173799</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1.33898716281177</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1.20866743770415</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1.1651028095365701</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1.1390817646872</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1.1249215439065601</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1.13900141343992</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1.0912231451293599</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1.1311208463048801</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1.3404605989048799</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1.0761014631298</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1.1392309384729999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1.06606395986014</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1.5478802937051801</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1.0562719363651401</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1.01422823626237</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1">
-        <v>1.0170810789507501</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1">
-        <v>1.01965479728596</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1">
-        <v>4.1247172070595601</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1">
+      <c r="C36">
         <v>1.0087471134881301</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1">
-        <v>1.2853214624389999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1">
-        <v>1.53282082393621</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>86</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1">
-        <v>1.1633175016633599</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>87</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1">
-        <v>0.85407147749781398</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>88</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1">
-        <v>1.4201301937451201</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>89</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1">
-        <v>1.9879225691309099</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1">
-        <v>1.2171219834114699</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>91</v>
-      </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1">
-        <v>2.3017252713169598</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>92</v>
-      </c>
+      <c r="C37">
+        <v>1.0084617378615699</v>
+      </c>
+      <c r="D37">
+        <v>16</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
-      <c r="C38" s="1">
-        <v>1.0084617378615699</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>93</v>
-      </c>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
-      <c r="C39" s="1">
-        <v>0.88086812302217299</v>
-      </c>
+      <c r="C39" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C39">
-    <sortCondition descending="1" ref="B1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E39">
+    <sortCondition descending="1" ref="C1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>